<commit_message>
feat: update requirements for right to left support
</commit_message>
<xml_diff>
--- a/data/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
+++ b/data/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/stimuli_toy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7CA67F-50EE-D240-B9AF-CB1A705D2B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4D8E84-D313-1642-84F0-501C493C47F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
+    <workbookView xWindow="42240" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="PopSci_MultiplEYE_EN_example_st" sheetId="2" r:id="rId1"/>
@@ -127,9 +127,6 @@
     <t>toy_text_1</t>
   </si>
   <si>
-    <t>pymovements</t>
-  </si>
-  <si>
     <t>ABSTRACT 
 pymovements: A Python package for eye movement data processing, ETRA 2023</t>
   </si>
@@ -140,9 +137,6 @@
     <t>toy_text_2</t>
   </si>
   <si>
-    <t>Eye-tracking</t>
-  </si>
-  <si>
     <t xml:space="preserve">Eye movements in reading are known to reflect cognitive processes involved in reading comprehension at all linguistic levels, from the sub-lexical to the discourse level. This means that reading comprehension and other properties of the text and/or the reader should be possible to infer from eye movements. Consequently, we develop the first neural sequence architecture for this type of tasks which models scan paths in reading and incorporates lexical, semantic and other linguistic features of the stimulus text. Our proposed model outperforms state-of-the-art models in various tasks. </t>
   </si>
   <si>
@@ -153,6 +147,12 @@
   </si>
   <si>
     <t>toy_text_3</t>
+  </si>
+  <si>
+    <t>Eye tracking</t>
+  </si>
+  <si>
+    <t>pymovements</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <dimension ref="A1:BU17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -870,13 +870,13 @@
         <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="X2"/>
       <c r="Y2"/>
@@ -914,16 +914,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="X3"/>
       <c r="Y3"/>
@@ -961,18 +961,18 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:73" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:73" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
feat: add block information to stimuli files
</commit_message>
<xml_diff>
--- a/data/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
+++ b/data/stimuli_toy/multipleye_stimuli_experiment_toy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/debor/repos/wg1-image-creation/data/stimuli_toy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4D8E84-D313-1642-84F0-501C493C47F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78FB5780-5295-B34C-A7F5-AD5DEF7703D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42240" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
+    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="18660" xr2:uid="{EF339F11-F4DE-4D0A-862E-E00578AF5D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="PopSci_MultiplEYE_EN_example_st" sheetId="2" r:id="rId1"/>
@@ -727,7 +727,7 @@
   <dimension ref="A1:BU17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -911,7 +911,7 @@
     </row>
     <row r="3" spans="1:73" ht="122.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>28</v>
@@ -958,7 +958,7 @@
     </row>
     <row r="4" spans="1:73" ht="128" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
         <v>32</v>

</xml_diff>